<commit_message>
changes Pused till 05 Aug
</commit_message>
<xml_diff>
--- a/SF_US/Data_Sheets/Data_Sheet.xlsx
+++ b/SF_US/Data_Sheets/Data_Sheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SFUS\AristocratGLBIT-SFUS\SF_US\Data_Sheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AristocratGLBIT-SFUS-Ashu_16_06_2025_V2\AristocratGLBIT-SFUS-Ashu_16_06_2025\SF_US\Data_Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4DBBAB6-4F23-4F59-8D3C-12ECD5A16D1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC6374CB-9ED8-40FF-9C92-5CA4F8D03230}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="SF_opportunity" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -406,7 +405,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -416,9 +415,10 @@
     <col min="4" max="4" width="14.08984375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.1796875" customWidth="1"/>
     <col min="6" max="6" width="19.36328125" customWidth="1"/>
-    <col min="7" max="7" width="13.6328125" customWidth="1"/>
-    <col min="8" max="8" width="10.36328125" customWidth="1"/>
-    <col min="10" max="10" width="12.90625" customWidth="1"/>
+    <col min="7" max="7" width="24" customWidth="1"/>
+    <col min="8" max="8" width="13" customWidth="1"/>
+    <col min="9" max="9" width="16.453125" customWidth="1"/>
+    <col min="10" max="10" width="18.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
@@ -493,6 +493,18 @@
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
       </c>
       <c r="F4" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
B01-B06 NEW CHANGES ON 14/08
</commit_message>
<xml_diff>
--- a/SF_US/Data_Sheets/Data_Sheet.xlsx
+++ b/SF_US/Data_Sheets/Data_Sheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AristocratGLBIT-SFUS-Ashu_16_06_2025_V2\AristocratGLBIT-SFUS-Ashu_16_06_2025\SF_US\Data_Sheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AristocratGLBIT-SFUS-Ashu_16_06_2025\SF_US\Data_Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC6374CB-9ED8-40FF-9C92-5CA4F8D03230}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8181B43A-8BBB-4530-BBB4-A9DEA57C7F5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -405,7 +405,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
C series changes pushed
</commit_message>
<xml_diff>
--- a/SF_US/Data_Sheets/Data_Sheet.xlsx
+++ b/SF_US/Data_Sheets/Data_Sheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AristocratGLBIT-SFUS-Ashu_16_06_2025\SF_US\Data_Sheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TestComplete_Namemapping\AristocratGLBIT-SFUS-Ashu_16_06_2025\SF_US\Data_Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8181B43A-8BBB-4530-BBB4-A9DEA57C7F5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1200299F-13E2-401D-AAAB-E2D0EAE26CCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -82,6 +82,66 @@
   </si>
   <si>
     <t>B04</t>
+  </si>
+  <si>
+    <t>C02</t>
+  </si>
+  <si>
+    <t>GameTheme</t>
+  </si>
+  <si>
+    <t>FAST</t>
+  </si>
+  <si>
+    <t>GameTitle</t>
+  </si>
+  <si>
+    <t>Topper</t>
+  </si>
+  <si>
+    <t>Denom</t>
+  </si>
+  <si>
+    <t>VAR</t>
+  </si>
+  <si>
+    <t>CandleColor</t>
+  </si>
+  <si>
+    <t>TicketValidation</t>
+  </si>
+  <si>
+    <t>AuditSwitch</t>
+  </si>
+  <si>
+    <t>ButtonPanel</t>
+  </si>
+  <si>
+    <t>UnitDisc</t>
+  </si>
+  <si>
+    <t>TIGER WEALTH - (GT-TIGER WEALTH)</t>
+  </si>
+  <si>
+    <t>TOPPER 19.5 INCH LCD HELIX XT LATAM - (TPP000127-LATAM|01)</t>
+  </si>
+  <si>
+    <t>BTN PANEL 13 LCD HELIX SLANT AND UPRIGHT REFURB - (TBTN000079|01)</t>
+  </si>
+  <si>
+    <t>.01 - (DENOM_3)</t>
+  </si>
+  <si>
+    <t>0 - (VAR_0)</t>
+  </si>
+  <si>
+    <t>FILM CANDLE BLANK PLATE CHAMPAGNE - (CAN000015|01)</t>
+  </si>
+  <si>
+    <t>NONE - USE OPTION WHEN THERE IS NO TKT - (TKV000011|01)</t>
+  </si>
+  <si>
+    <t>2341 Audit Switch - IGT Flat Key - (AUDSW_3)</t>
   </si>
 </sst>
 </file>
@@ -402,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:T5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="S5" sqref="S5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -421,7 +481,7 @@
     <col min="10" max="10" width="18.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -452,8 +512,38 @@
       <c r="J1" t="s">
         <v>17</v>
       </c>
+      <c r="K1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>26</v>
+      </c>
+      <c r="R1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S1" t="s">
+        <v>28</v>
+      </c>
+      <c r="T1" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -473,7 +563,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -490,7 +580,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -508,6 +598,41 @@
       </c>
       <c r="F4" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L5" t="s">
+        <v>31</v>
+      </c>
+      <c r="M5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N5" t="s">
+        <v>33</v>
+      </c>
+      <c r="O5" t="s">
+        <v>34</v>
+      </c>
+      <c r="P5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>36</v>
+      </c>
+      <c r="R5" t="s">
+        <v>37</v>
+      </c>
+      <c r="S5" t="s">
+        <v>38</v>
+      </c>
+      <c r="T5">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>